<commit_message>
Scale function remove + Chinese Translate
</commit_message>
<xml_diff>
--- a/Resources/data-template(Chinese).xlsx
+++ b/Resources/data-template(Chinese).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CompanyProjects\mixer-control-globalver\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654F0308-9D50-4011-8880-3965E53031B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B6D9EE-7E0A-4CF0-ACB1-E70D4B14CA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F16F4896-5A00-4506-B4C6-D29130D26770}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Mã nguyên vật liệu
 原料编码</t>
@@ -55,10 +55,6 @@
   <si>
     <t>Mô tả bước
 操作内容</t>
-  </si>
-  <si>
-    <t>Đơn vị thực tế
-实际使用单位</t>
   </si>
   <si>
     <t>Trọng lượng (kg)
@@ -218,6 +214,49 @@
     </r>
     <r>
       <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Các cột có màu vàng là các giá trị </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BẮT BUỘC</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, các giá trị còn lại có thể bỏ trống.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
         <b/>
         <u/>
         <sz val="14"/>
@@ -226,208 +265,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>- Đơn vị thực thế:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>KG :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Khi nguyên vật liệu cần phải đo trọng lượng.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Packed :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Nguyên vật liệu tính bằng số gói </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(không đo trọng lượng).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- Các cột có màu vàng là các giá trị </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>BẮT BUỘC</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, các giá trị còn lại có thể bỏ trống.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>*注解 :</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>- 实际使用单位:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-KG (公斤): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>原料要过磅时</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Packed (包): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">原料按包来计算重量 </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">(不要过磅)。
-</t>
     </r>
     <r>
       <rPr>
@@ -958,7 +796,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43F945A8-7C13-4EDA-B471-5349D355352A}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -971,14 +809,13 @@
     <col min="3" max="3" width="19.5546875" style="4" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="18.44140625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.44140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="9.33203125" style="5" customWidth="1"/>
-    <col min="8" max="10" width="8.88671875" style="1"/>
-    <col min="11" max="11" width="48.5546875" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="1"/>
+    <col min="6" max="6" width="9.33203125" style="5" customWidth="1"/>
+    <col min="7" max="9" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="48.5546875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="44.25" customHeight="1">
+    <row r="1" spans="1:10" ht="44.25" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>1</v>
       </c>
@@ -989,210 +826,193 @@
         <v>2</v>
       </c>
       <c r="D1" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>15</v>
-      </c>
+      <c r="F1" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="27"/>
       <c r="H1" s="27"/>
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-    </row>
-    <row r="2" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="2" spans="1:10" ht="19.95" customHeight="1">
       <c r="A2" s="17"/>
       <c r="B2" s="18"/>
       <c r="C2" s="19"/>
       <c r="D2" s="21"/>
       <c r="E2" s="20"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="27"/>
       <c r="I2" s="27"/>
       <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-    </row>
-    <row r="3" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="3" spans="1:10" ht="19.95" customHeight="1">
       <c r="A3" s="17"/>
       <c r="B3" s="18"/>
       <c r="C3" s="19"/>
       <c r="D3" s="21"/>
       <c r="E3" s="20"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="27"/>
       <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
-    </row>
-    <row r="4" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="4" spans="1:10" ht="19.95" customHeight="1">
       <c r="A4" s="17"/>
       <c r="B4" s="18"/>
       <c r="C4" s="19"/>
       <c r="D4" s="21"/>
       <c r="E4" s="20"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="27"/>
       <c r="H4" s="27"/>
       <c r="I4" s="27"/>
       <c r="J4" s="27"/>
-      <c r="K4" s="27"/>
-    </row>
-    <row r="5" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="5" spans="1:10" ht="19.95" customHeight="1">
       <c r="A5" s="17"/>
       <c r="B5" s="18"/>
       <c r="C5" s="19"/>
       <c r="D5" s="21"/>
       <c r="E5" s="20"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27"/>
       <c r="H5" s="27"/>
       <c r="I5" s="27"/>
       <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-    </row>
-    <row r="6" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="6" spans="1:10" ht="19.95" customHeight="1">
       <c r="A6" s="17"/>
       <c r="B6" s="18"/>
       <c r="C6" s="19"/>
       <c r="D6" s="21"/>
       <c r="E6" s="20"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27"/>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-    </row>
-    <row r="7" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="7" spans="1:10" ht="19.95" customHeight="1">
       <c r="A7" s="17"/>
       <c r="B7" s="18"/>
       <c r="C7" s="19"/>
       <c r="D7" s="21"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27"/>
       <c r="H7" s="27"/>
       <c r="I7" s="27"/>
       <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-    </row>
-    <row r="8" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="8" spans="1:10" ht="19.95" customHeight="1">
       <c r="A8" s="17"/>
       <c r="B8" s="18"/>
       <c r="C8" s="19"/>
       <c r="D8" s="21"/>
       <c r="E8" s="20"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="27"/>
       <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-    </row>
-    <row r="9" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="9" spans="1:10" ht="19.95" customHeight="1">
       <c r="A9" s="17"/>
       <c r="B9" s="18"/>
       <c r="C9" s="19"/>
       <c r="D9" s="21"/>
       <c r="E9" s="20"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
       <c r="H9" s="27"/>
       <c r="I9" s="27"/>
       <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-    </row>
-    <row r="10" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="10" spans="1:10" ht="19.95" customHeight="1">
       <c r="A10" s="17"/>
       <c r="B10" s="18"/>
       <c r="C10" s="19"/>
       <c r="D10" s="21"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="27"/>
       <c r="I10" s="27"/>
       <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-    </row>
-    <row r="11" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="11" spans="1:10" ht="19.95" customHeight="1">
       <c r="A11" s="17"/>
       <c r="B11" s="18"/>
       <c r="C11" s="19"/>
       <c r="D11" s="21"/>
       <c r="E11" s="20"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="27"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
       <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-    </row>
-    <row r="12" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="12" spans="1:10" ht="19.95" customHeight="1">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
       <c r="D12" s="21"/>
       <c r="E12" s="20"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="27"/>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
-      <c r="K12" s="27"/>
-    </row>
-    <row r="13" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="13" spans="1:10" ht="19.95" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
       <c r="D13" s="21"/>
       <c r="E13" s="20"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="27"/>
       <c r="I13" s="27"/>
       <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-    </row>
-    <row r="14" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="14" spans="1:10" ht="19.95" customHeight="1">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
       <c r="D14" s="21"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27"/>
       <c r="H14" s="27"/>
       <c r="I14" s="27"/>
       <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-    </row>
-    <row r="15" spans="1:11" ht="19.95" customHeight="1">
+    </row>
+    <row r="15" spans="1:10" ht="19.95" customHeight="1">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="21"/>
       <c r="E15" s="20"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27"/>
       <c r="H15" s="27"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G1:K15"/>
+    <mergeCell ref="F1:J15"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 G16:G1048576" xr:uid="{5448CEC1-C1FA-4C22-A2C6-E9BC80840D45}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16:F1048576" xr:uid="{5448CEC1-C1FA-4C22-A2C6-E9BC80840D45}">
       <formula1>"KG,Packed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1226,22 +1046,22 @@
   <sheetData>
     <row r="1" spans="1:12" ht="74.400000000000006" customHeight="1">
       <c r="A1" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="E1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="12" t="s">
         <v>12</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>13</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>3</v>
@@ -1250,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>

</xml_diff>

<commit_message>
Change start and reset logics
- Start at each step & reset logic when change to other tab/ close the application
</commit_message>
<xml_diff>
--- a/Resources/data-template(Chinese).xlsx
+++ b/Resources/data-template(Chinese).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CompanyProjects\mixer-control-globalver\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B6D9EE-7E0A-4CF0-ACB1-E70D4B14CA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C12A92E-EC5A-4E9E-BB4B-442DCD985B4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F16F4896-5A00-4506-B4C6-D29130D26770}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F16F4896-5A00-4506-B4C6-D29130D26770}"/>
   </bookViews>
   <sheets>
     <sheet name="material_info" sheetId="1" r:id="rId1"/>
@@ -85,10 +85,6 @@
 第二段运行时间 (分钟)</t>
   </si>
   <si>
-    <t>Hút chân không
-抽监控</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -278,6 +274,10 @@
       <t xml:space="preserve">
 - 黄色列为必填项，其他列为选填项。</t>
     </r>
+  </si>
+  <si>
+    <t>Hút chân không
+抽真空</t>
   </si>
 </sst>
 </file>
@@ -832,7 +832,7 @@
         <v>6</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G1" s="27"/>
       <c r="H1" s="27"/>
@@ -1026,7 +1026,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:L15"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1061,7 +1061,7 @@
         <v>11</v>
       </c>
       <c r="F1" s="12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>3</v>
@@ -1070,7 +1070,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="29"/>
       <c r="K1" s="29"/>

</xml_diff>